<commit_message>
[YD]added the backend import funcitonlity added the discount to portal view raise error if partner does not contain sales team or pricelist
[RK]
use the product price unit instead of excel price price unit
</commit_message>
<xml_diff>
--- a/sale_portal_extended/static/src/document/order.xlsx
+++ b/sale_portal_extended/static/src/document/order.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRODUCT</t>
   </si>
   <si>
@@ -49,9 +46,6 @@
     <t xml:space="preserve">DESCRIPTION</t>
   </si>
   <si>
-    <t xml:space="preserve">price_unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">8904256305006</t>
   </si>
   <si>
@@ -67,27 +61,15 @@
     <t xml:space="preserve">DESK0006</t>
   </si>
   <si>
-    <t xml:space="preserve">230</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">560</t>
-  </si>
-  <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">240</t>
-  </si>
-  <si>
     <t xml:space="preserve">E-COM11</t>
   </si>
   <si>
-    <t xml:space="preserve">360</t>
-  </si>
-  <si>
     <t xml:space="preserve">8904256305007</t>
   </si>
   <si>
@@ -95,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Product B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234</t>
   </si>
 </sst>
 </file>
@@ -180,31 +159,30 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -220,127 +198,103 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>